<commit_message>
New taaaaaasks and edited intro
</commit_message>
<xml_diff>
--- a/Project Work/Writing.xlsx
+++ b/Project Work/Writing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>Subject</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Oliver</t>
   </si>
   <si>
-    <t>Done?</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -116,10 +113,43 @@
     <t xml:space="preserve"> - Materials</t>
   </si>
   <si>
-    <t xml:space="preserve"> - Procedure</t>
-  </si>
-  <si>
     <t>Haagh</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Procedure(s)</t>
+  </si>
+  <si>
+    <t>Read?</t>
+  </si>
+  <si>
+    <t>Extra Work</t>
+  </si>
+  <si>
+    <t>Introduction fix table</t>
+  </si>
+  <si>
+    <t>Source on price of RAMIS</t>
+  </si>
+  <si>
+    <t>Include tools in Artefact model</t>
+  </si>
+  <si>
+    <t>Interview conclusions</t>
+  </si>
+  <si>
+    <t>Add Johan's interview</t>
+  </si>
+  <si>
+    <t>Rewrite rules</t>
+  </si>
+  <si>
+    <t>Merge interviews and obs.</t>
+  </si>
+  <si>
+    <t>Nicklas</t>
+  </si>
+  <si>
+    <t>Freddie</t>
   </si>
 </sst>
 </file>
@@ -490,15 +520,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70EBFDB9-AC42-4B2C-A0DE-44911FC47DD6}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
   </cols>
@@ -514,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -527,10 +557,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="3">
         <v>43036</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,7 +581,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
         <v>43036</v>
@@ -579,10 +612,13 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3">
         <v>43036</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3">
         <v>43036</v>
@@ -612,7 +648,7 @@
         <v>43036</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -626,7 +662,7 @@
         <v>43036</v>
       </c>
       <c r="D16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -640,7 +676,7 @@
         <v>43036</v>
       </c>
       <c r="D17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,17 +686,17 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -672,10 +708,93 @@
       <c r="A23" t="s">
         <v>17</v>
       </c>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>33</v>
+      </c>
+      <c r="B27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C31" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="3">
+        <v>43042</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="3">
+        <v>43042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more methods, added second article tab in writing for more work
</commit_message>
<xml_diff>
--- a/Project Work/Writing.xlsx
+++ b/Project Work/Writing.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>Subject</t>
   </si>
@@ -189,6 +189,15 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>Article Continued</t>
+  </si>
+  <si>
+    <t>Should we have more intro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - This could be about the robot itself</t>
   </si>
 </sst>
 </file>
@@ -604,7 +613,7 @@
   <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,8 +823,11 @@
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J16" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -828,8 +840,14 @@
       <c r="D17" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>56</v>
+      </c>
+      <c r="L17" s="3">
+        <v>43059</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -842,8 +860,11 @@
       <c r="D18" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -857,12 +878,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -873,7 +894,7 @@
         <v>43049</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -884,7 +905,7 @@
         <v>43049</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -898,7 +919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -912,7 +933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -923,17 +944,17 @@
         <v>43049</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>30</v>
       </c>
@@ -947,7 +968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>31</v>
       </c>
@@ -961,7 +982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Did all my things
</commit_message>
<xml_diff>
--- a/Project Work/Writing.xlsx
+++ b/Project Work/Writing.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicki\Documents\surgeon_sim_vr\Project Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niclas\Documents\UNI\VGIS7\Projekt\Project Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -744,21 +744,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="10" max="10" width="34.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.54296875" customWidth="1"/>
+    <col min="10" max="10" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -772,12 +772,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
@@ -803,7 +803,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -820,7 +820,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -831,7 +831,7 @@
         <v>43062</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -848,7 +848,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -868,7 +868,7 @@
         <v>43070</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -879,7 +879,7 @@
         <v>43060</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -887,7 +887,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
@@ -901,12 +901,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
@@ -929,7 +929,7 @@
         <v>43061</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -940,7 +940,7 @@
         <v>43036</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J14" s="4" t="s">
         <v>52</v>
       </c>
@@ -951,7 +951,7 @@
         <v>43087</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -959,7 +959,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -983,7 +983,7 @@
       </c>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>18</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>43059</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>43059</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>43059</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>24</v>
       </c>
@@ -1074,7 +1074,7 @@
         <v>43059</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>43049</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1121,17 +1121,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J28" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
         <v>63</v>
       </c>
@@ -1140,7 +1140,7 @@
       </c>
       <c r="L29" s="3"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J30" t="s">
         <v>65</v>
       </c>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
         <v>67</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
         <v>68</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>29</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
         <v>31</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>32</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>36</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
         <v>33</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>34</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>35</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
         <v>39</v>
       </c>
@@ -1321,12 +1321,12 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>80</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>81</v>
       </c>
@@ -1359,29 +1359,29 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C48" s="3">
-        <v>43083</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" t="s">
+      <c r="C48" s="7">
+        <v>43083</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C49" s="3">
-        <v>43083</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C49" s="7">
+        <v>43083</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>83</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>84</v>
       </c>
@@ -1399,7 +1399,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -1410,18 +1410,18 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C53" s="3">
-        <v>43083</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C53" s="7">
+        <v>43083</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>87</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>88</v>
       </c>
@@ -1443,7 +1443,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>89</v>
       </c>
@@ -1454,7 +1454,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>90</v>
       </c>
@@ -1465,7 +1465,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>91</v>
       </c>
@@ -1476,7 +1476,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>92</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>93</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>94</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>95</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>96</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -1542,14 +1542,14 @@
         <v>43083</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C65" s="3">
+      <c r="C65" s="5">
         <v>43083</v>
       </c>
     </row>

</xml_diff>